<commit_message>
some corrections from regression testing. process disabling and acquirable material testing in progress.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/warehouse_with_entry_processes_modify_test_cases.xlsx
+++ b/soberano/test_cases/warehouse_with_entry_processes_modify_test_cases.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">pr2,pr3</t>
+    <t xml:space="preserve">mpr2,mpr3</t>
   </si>
   <si>
     <t xml:space="preserve">User2 is allowed to modify warehouse</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">mw22</t>
   </si>
   <si>
-    <t xml:space="preserve">pr2,pr4</t>
+    <t xml:space="preserve">mpr2,mpr4</t>
   </si>
   <si>
     <t xml:space="preserve">User3 is allowed to modify warehouse</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">mw23</t>
   </si>
   <si>
-    <t xml:space="preserve">pr4,pr5,pr7</t>
+    <t xml:space="preserve">mpr4,mpr5,mpr7</t>
   </si>
   <si>
     <t xml:space="preserve">User4 is NOT allowed to modify warehouse</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">mw24</t>
   </si>
   <si>
-    <t xml:space="preserve">pr8,pr9,pr10</t>
+    <t xml:space="preserve">mpr8,mpr9,mpr10</t>
   </si>
   <si>
     <t xml:space="preserve">User5 is NOT allowed to modify warehouse</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">mw26</t>
   </si>
   <si>
-    <t xml:space="preserve">pr2,pr3,pr4</t>
+    <t xml:space="preserve">mpr2,mpr3,mpr4</t>
   </si>
   <si>
     <t xml:space="preserve">User9 is allowed to modify warehouse</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">mw27</t>
   </si>
   <si>
-    <t xml:space="preserve">pr4,pr5</t>
+    <t xml:space="preserve">mpr4,mpr5</t>
   </si>
   <si>
     <t xml:space="preserve">User11 is allowed to modify warehouse</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">mw28</t>
   </si>
   <si>
-    <t xml:space="preserve">Pr6,pr7,pr8,pr9</t>
+    <t xml:space="preserve">mpr6,mpr7,mpr8,mpr9</t>
   </si>
   <si>
     <t xml:space="preserve">User12 is allowed to modify warehouse</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">mw29</t>
   </si>
   <si>
-    <t xml:space="preserve">pr3</t>
+    <t xml:space="preserve">mpr3</t>
   </si>
   <si>
     <t xml:space="preserve">User13 NOT is allowed to modify warehouse</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">mw30</t>
   </si>
   <si>
-    <t xml:space="preserve">pr3,pr4,pr5</t>
+    <t xml:space="preserve">mpr3,mpr4,mpr5</t>
   </si>
   <si>
     <t xml:space="preserve">User14 is NOT allowed to modify warehouse</t>
@@ -351,7 +351,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
unstable. material expense coding half way.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/warehouse_with_entry_processes_modify_test_cases.xlsx
+++ b/soberano/test_cases/warehouse_with_entry_processes_modify_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">mpr2,mpr3</t>
+    <t xml:space="preserve">mpr2,mpr4</t>
   </si>
   <si>
     <t xml:space="preserve">User2 is allowed to modify warehouse</t>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">mw22</t>
   </si>
   <si>
-    <t xml:space="preserve">mpr2,mpr4</t>
-  </si>
-  <si>
     <t xml:space="preserve">User3 is allowed to modify warehouse</t>
   </si>
   <si>
@@ -157,7 +154,7 @@
     <t xml:space="preserve">mw29</t>
   </si>
   <si>
-    <t xml:space="preserve">mpr3</t>
+    <t xml:space="preserve">mpr4</t>
   </si>
   <si>
     <t xml:space="preserve">User13 NOT is allowed to modify warehouse</t>
@@ -351,7 +348,7 @@
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,7 +444,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,22 +452,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,22 +475,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,22 +498,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,22 +521,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,13 +544,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
@@ -567,22 +564,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,22 +587,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,22 +610,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,22 +633,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,22 +656,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,22 +679,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,22 +702,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,22 +725,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +748,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,7 +756,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,7 +772,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,7 +788,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,7 +796,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,7 +804,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +812,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +820,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>